<commit_message>
combined redundant/similar/vague taxa in time series data
</commit_message>
<xml_diff>
--- a/data/TL_empirical_species.xlsx
+++ b/data/TL_empirical_species.xlsx
@@ -1562,8 +1562,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F168" sqref="F168:F170"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A127" sqref="A127:XFD128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
matched taxa names w/ time series & web stats
</commit_message>
<xml_diff>
--- a/data/TL_empirical_species.xlsx
+++ b/data/TL_empirical_species.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="238">
   <si>
     <t>name</t>
   </si>
@@ -725,6 +725,9 @@
   </si>
   <si>
     <t>Decent time series data</t>
+  </si>
+  <si>
+    <t>Good time series 1984-85; 1989-90</t>
   </si>
 </sst>
 </file>
@@ -1562,8 +1565,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A127" sqref="A127:XFD128"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G166" sqref="G166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4489,7 +4492,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>144</v>
       </c>
@@ -4500,7 +4503,13 @@
         <v>129</v>
       </c>
       <c r="D162">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G162" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>